<commit_message>
05.01.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/January/All Details/04.01.2020/MC Bank Statement Jan'2020.xlsx
+++ b/2020/January/All Details/04.01.2020/MC Bank Statement Jan'2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\January\All Details\04.01.2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD26DEF-2345-41BD-8159-0CCD178204D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAAF953-C19F-4B16-8CAF-041B59E2C79A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-210" yWindow="555" windowWidth="14310" windowHeight="9990" tabRatio="599" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="December" sheetId="7" r:id="rId1"/>
@@ -3052,7 +3052,7 @@
   <dimension ref="A1:AK222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" customHeight="1"/>

</xml_diff>